<commit_message>
Razorpay payment screen changes fixed
</commit_message>
<xml_diff>
--- a/Reports/Graph_Sprint_Data/UI_RazorPay_REGISTRATION_HISTORY_DATA.xlsx
+++ b/Reports/Graph_Sprint_Data/UI_RazorPay_REGISTRATION_HISTORY_DATA.xlsx
@@ -478,7 +478,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:G10"/>
@@ -1310,6 +1310,60 @@
       </c>
       <c r="G30" s="5" t="n">
         <v>1.27</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="5" t="inlineStr">
+        <is>
+          <t>2023-02-07</t>
+        </is>
+      </c>
+      <c r="B31" s="10" t="n">
+        <v>44964.49304700232</v>
+      </c>
+      <c r="C31" s="5" t="inlineStr">
+        <is>
+          <t>testingpay172</t>
+        </is>
+      </c>
+      <c r="D31" s="5" t="n">
+        <v>41</v>
+      </c>
+      <c r="E31" s="5" t="n">
+        <v>42</v>
+      </c>
+      <c r="F31" s="5" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G31" s="5" t="n">
+        <v>1.56</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="5" t="inlineStr">
+        <is>
+          <t>2023-02-07</t>
+        </is>
+      </c>
+      <c r="B32" s="10" t="n">
+        <v>44964.50708280093</v>
+      </c>
+      <c r="C32" s="5" t="inlineStr">
+        <is>
+          <t>ppaytest1172</t>
+        </is>
+      </c>
+      <c r="D32" s="5" t="n">
+        <v>44</v>
+      </c>
+      <c r="E32" s="5" t="n">
+        <v>43</v>
+      </c>
+      <c r="F32" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G32" s="5" t="n">
+        <v>2.3</v>
       </c>
     </row>
   </sheetData>
@@ -1626,7 +1680,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:G10"/>
@@ -2374,30 +2428,84 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr">
+      <c r="A28" s="5" t="inlineStr">
         <is>
           <t>2023-02-03</t>
         </is>
       </c>
       <c r="B28" s="10" t="n">
-        <v>44960.63808569634</v>
-      </c>
-      <c r="C28" t="inlineStr">
+        <v>44960.63808569445</v>
+      </c>
+      <c r="C28" s="5" t="inlineStr">
         <is>
           <t>pay172three</t>
         </is>
       </c>
-      <c r="D28" t="n">
-        <v>41</v>
-      </c>
-      <c r="E28" t="n">
+      <c r="D28" s="5" t="n">
+        <v>41</v>
+      </c>
+      <c r="E28" s="5" t="n">
         <v>39</v>
       </c>
-      <c r="F28" t="n">
+      <c r="F28" s="5" t="n">
         <v>2</v>
       </c>
-      <c r="G28" t="n">
+      <c r="G28" s="5" t="n">
         <v>1.03</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="5" t="inlineStr">
+        <is>
+          <t>2023-02-07</t>
+        </is>
+      </c>
+      <c r="B29" s="10" t="n">
+        <v>44964.5041196875</v>
+      </c>
+      <c r="C29" s="5" t="inlineStr">
+        <is>
+          <t>testingpay172</t>
+        </is>
+      </c>
+      <c r="D29" s="5" t="n">
+        <v>44</v>
+      </c>
+      <c r="E29" s="5" t="n">
+        <v>43</v>
+      </c>
+      <c r="F29" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G29" s="5" t="n">
+        <v>1.56</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2023-02-07</t>
+        </is>
+      </c>
+      <c r="B30" s="10" t="n">
+        <v>44964.57731602514</v>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>testff172</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>44</v>
+      </c>
+      <c r="E30" t="n">
+        <v>44</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0</v>
+      </c>
+      <c r="G30" t="n">
+        <v>1.36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>